<commit_message>
Updated and finished for tonight 1-31
</commit_message>
<xml_diff>
--- a/Database Model.xlsx
+++ b/Database Model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19980" windowHeight="9345"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19980" windowHeight="9345" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Conceptual Model" sheetId="2" r:id="rId1"/>
@@ -65,6 +65,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDCFF85"/>
+      <color rgb="FFFDD49D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1945,8 +1951,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>560120</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>121227</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1957,8 +1963,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5323485" y="3856450"/>
-          <a:ext cx="2510271" cy="455777"/>
+          <a:off x="5351194" y="3856450"/>
+          <a:ext cx="2524126" cy="544100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1996,6 +2002,20 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
+            <a:t>Transaction ID</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
             <a:t>Card ID</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -2027,14 +2047,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>474394</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>139972</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>560120</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
+      <xdr:rowOff>95252</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2045,8 +2065,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5323485" y="4330972"/>
-          <a:ext cx="2510271" cy="812530"/>
+          <a:off x="5351194" y="4410075"/>
+          <a:ext cx="2524126" cy="828677"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2526,13 +2546,13 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>402771</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>488496</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>17317</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2543,8 +2563,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13404396" y="5610225"/>
-          <a:ext cx="2562225" cy="609600"/>
+          <a:off x="13131635" y="5610224"/>
+          <a:ext cx="2510270" cy="693593"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2585,14 +2605,8 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>Event ID</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:latin typeface="Calibri"/>
-          </a:endParaRPr>
+            <a:t>Attendance ID</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
@@ -2608,7 +2622,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>Member ID</a:t>
+            <a:t>Event ID</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
@@ -2631,7 +2645,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t> </a:t>
+            <a:t>Member ID</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
@@ -2656,6 +2670,29 @@
             </a:rPr>
             <a:t> </a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2666,13 +2703,13 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>402771</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>185304</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>488496</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>109104</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2683,8 +2720,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="13404396" y="6229350"/>
-          <a:ext cx="2562225" cy="304800"/>
+          <a:off x="13131635" y="6281304"/>
+          <a:ext cx="2510270" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2986,6 +3023,20 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
+            <a:t>MemberNumber</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
             <a:t>First Name</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -3126,7 +3177,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>Current</a:t>
+            <a:t>CurrentFlag</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
@@ -4172,7 +4223,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>Current</a:t>
+            <a:t>CurrentFlag</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
@@ -4668,13 +4719,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>474395</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>37605</xdr:rowOff>
+      <xdr:rowOff>37604</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>528824</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>83839</xdr:rowOff>
+      <xdr:rowOff>127999</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4686,8 +4737,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="5323486" y="1752105"/>
-          <a:ext cx="54429" cy="2332234"/>
+          <a:off x="5351195" y="1752104"/>
+          <a:ext cx="54429" cy="2376395"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -4778,7 +4829,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>436789</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>51521</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4791,7 +4842,7 @@
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
           <a:off x="13131635" y="4073979"/>
-          <a:ext cx="34018" cy="1841046"/>
+          <a:ext cx="34018" cy="1883042"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -4830,7 +4881,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>402771</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>51520</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4843,7 +4894,7 @@
       <xdr:spPr>
         <a:xfrm rot="10800000" flipH="1" flipV="1">
           <a:off x="9207707" y="3107871"/>
-          <a:ext cx="3923928" cy="2807153"/>
+          <a:ext cx="3923928" cy="2849149"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -5021,6 +5072,4463 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>527958</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>269918</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>172316</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Text Box 2"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8394487" y="4039466"/>
+          <a:ext cx="1557313" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>PaymentCard</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>54429</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>172316</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>126300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19916</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Text Box 6"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7979229" y="4363316"/>
+          <a:ext cx="2510271" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CardID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (PK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MemberID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (FK) </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>54429</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>29441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>126300</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>124691</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Text Box 7"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7979229" y="4982441"/>
+          <a:ext cx="2510271" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CardType</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(45)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CardNumber</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(20)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CardExpiration</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> date</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>276102</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>189139</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>11258</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>131989</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Text Box 8"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16125702" y="3808639"/>
+          <a:ext cx="1563956" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Renewal</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>422441</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>131989</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>494312</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>112939</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="Text Box 9"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15662441" y="4132489"/>
+          <a:ext cx="2510271" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>RenewalID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (PK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>422441</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>122464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>494312</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>112939</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Text Box 10"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15662441" y="4503964"/>
+          <a:ext cx="2510271" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>RenewalType</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(15)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>RenewalPrice</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> smallmoney</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>480332</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>162111</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>215488</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104961</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Text Box 11"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8405132" y="6448611"/>
+          <a:ext cx="1563956" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Transactions</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>71871</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>136071</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Text Box 12"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7960179" y="6772461"/>
+          <a:ext cx="2521156" cy="602610"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>TransactionID </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>int (PK)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CardID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (FK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>144053</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>71871</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>4083</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Text Box 13"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7960179" y="7383053"/>
+          <a:ext cx="2521156" cy="812530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1300"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>TransactionDate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> date</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1300"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Charge</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> smallmoney</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1300"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Result</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(10)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>380628</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>115784</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>65315</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Text Box 14"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16230228" y="6408965"/>
+          <a:ext cx="1563956" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Events</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>526968</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>65315</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>598838</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>8165</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Text Box 15"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15766968" y="6732815"/>
+          <a:ext cx="2510270" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1300"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>EventID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (PK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1300"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>HostID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (FK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1300"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>526968</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>8165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>598838</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>189140</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Text Box 16"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15766968" y="7247165"/>
+          <a:ext cx="2510270" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1300"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>EventName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(100)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1300"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>EventDate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> date</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>339807</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>10886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>81767</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>144236</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Text Box 17"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16189407" y="8202386"/>
+          <a:ext cx="1570760" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>EventAttendance</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>492950</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>144235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>564820</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Text Box 18"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15732950" y="8526235"/>
+          <a:ext cx="2510270" cy="665389"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>AttendanceID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (PK)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>EventID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (FK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MemberID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(5) (FK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:lnSpc>
+              <a:spcPts val="1500"/>
+            </a:lnSpc>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>492950</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>564820</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Text Box 19"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15732950" y="9192986"/>
+          <a:ext cx="2510270" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>PresentStatus</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> bit</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>90551</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>85045</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>442112</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>27895</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="Text Box 20"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12282551" y="5419045"/>
+          <a:ext cx="1570761" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Members</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226622</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>27895</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>298494</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>18370</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Text Box 21"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11809022" y="5742895"/>
+          <a:ext cx="2510272" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MemberID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (PK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>RenewalID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (FK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226622</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>18370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>298494</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>189820</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="Text Box 22"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11809022" y="6304870"/>
+          <a:ext cx="2510272" cy="2266950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MemberNumber </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>varchar(10)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>FirstName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MiddleName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>LastName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Email</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(30)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Phone</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(15)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Gender </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>varchar(10)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>StartDate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> date</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CurrentFlag</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> bit</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>BirthDate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> date</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>42924</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>170770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>394485</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>113620</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Text Box 26"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12234924" y="8933770"/>
+          <a:ext cx="1570761" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MemberAddress</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>178995</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>113620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>250867</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>104095</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Text Box 27"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11761395" y="9257620"/>
+          <a:ext cx="2510272" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>AddressID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (PK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MemberID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int(FK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>178995</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>104095</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>250867</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>161245</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="Text Box 28"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11761395" y="9819595"/>
+          <a:ext cx="2510272" cy="1581150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>AddressType</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>AddressLine1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>AddressLine2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>City</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(35)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>StateProvince</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(25)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>PostalCode</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(15)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>166008</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>540082</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Text Box 26"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12268361" y="3429000"/>
+          <a:ext cx="1584309" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MemberInterest</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>324592</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>396464</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>51707</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="Text Box 27"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11906992" y="3752850"/>
+          <a:ext cx="2510272" cy="299357"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MemberID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (PK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>324592</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>52832</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>396464</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>155831</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="Text Box 28"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11906992" y="4053332"/>
+          <a:ext cx="2510272" cy="864999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Interest1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(20)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Interest2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(20)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Interest3</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(20)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>495978</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>21151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>237939</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>154501</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Text Box 20"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="20003178" y="5736151"/>
+          <a:ext cx="1570761" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Host</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>42242</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>154501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>100533</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>82324</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Text Box 21"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="19549442" y="6060001"/>
+          <a:ext cx="2496691" cy="308823"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>HostID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (PK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>55849</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>90548</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>114140</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>71498</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Text Box 22"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="19563049" y="6377048"/>
+          <a:ext cx="2496691" cy="2266950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>FirstName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>MiddleName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>LastName</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Email</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(30)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Phone</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(15)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Gender</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(10)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>StartDate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> date</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>CurrentFlag</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> bit</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>BirthDate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> date</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>576572</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165328</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>318532</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>108178</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Text Box 23"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="23131772" y="6261328"/>
+          <a:ext cx="1570760" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>HostAddress</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>107126</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>108178</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>178996</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>98653</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Text Box 24"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="22662326" y="6585178"/>
+          <a:ext cx="2510270" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FDD49D"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>AddressID </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>int (PK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>HostID</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> int (FK)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>107126</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>98653</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>178996</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>7486</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Text Box 25"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="22662326" y="7147153"/>
+          <a:ext cx="2510270" cy="1242333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="DCFF85"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>AddressLine1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>AddressLine2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(50)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>City</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(35)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>StateProvince</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(25)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>PostalCode</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> varchar(15)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>598838</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>118412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>42242</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>131989</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Elbow Connector 70"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="66" idx="1"/>
+          <a:endCxn id="51" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="18277238" y="6214412"/>
+          <a:ext cx="1272204" cy="775577"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>100533</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>118413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>107126</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>8166</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="Elbow Connector 71"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="66" idx="3"/>
+          <a:endCxn id="69" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22046133" y="6214413"/>
+          <a:ext cx="616193" cy="651753"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>96116</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>54430</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>25266</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Elbow Connector 72"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="42" idx="1"/>
+          <a:endCxn id="48" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="7960180" y="4668116"/>
+          <a:ext cx="54429" cy="2405650"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 519997"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>178996</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>118382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226623</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="74" name="Elbow Connector 73"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="57" idx="1"/>
+          <a:endCxn id="60" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="11761396" y="6023882"/>
+          <a:ext cx="47627" cy="3514725"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 579980"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>492950</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>131990</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>526968</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95930</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="Elbow Connector 74"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="51" idx="1"/>
+          <a:endCxn id="54" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="15732950" y="6989990"/>
+          <a:ext cx="34018" cy="1868940"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 771997"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226622</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>118382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>492950</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95929</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="Elbow Connector 75"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="57" idx="1"/>
+          <a:endCxn id="54" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="11809022" y="6023882"/>
+          <a:ext cx="3923928" cy="2835047"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -5826"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226622</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>92529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>324592</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>118383</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="Elbow Connector 76"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="57" idx="1"/>
+          <a:endCxn id="63" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="11809022" y="3902529"/>
+          <a:ext cx="97970" cy="2121354"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -233337"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>298495</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>122463</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>422442</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>118382</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Elbow Connector 77"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="45" idx="1"/>
+          <a:endCxn id="57" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="14319295" y="4313463"/>
+          <a:ext cx="1343147" cy="1710419"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>126300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>96117</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226622</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>118384</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Elbow Connector 78"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="57" idx="1"/>
+          <a:endCxn id="42" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="10489500" y="4668117"/>
+          <a:ext cx="1319522" cy="1355767"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>383758</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>134</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>305067</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152957</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="Text Box 11"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12506485" y="1905134"/>
+          <a:ext cx="1133582" cy="533823"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>LEGEND</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>331011</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>150165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>402882</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>162994</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="88" name="Text Box 13"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11847602" y="2436165"/>
+          <a:ext cx="2496416" cy="584329"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>NULL = RED</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>NOT NULL = BLACK </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5315,8 +9823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5331,8 +9839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J12:AB39"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5356,10 +9864,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Done for tonigt 2/1/2018
</commit_message>
<xml_diff>
--- a/Database Model.xlsx
+++ b/Database Model.xlsx
@@ -5352,7 +5352,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t> varchar(45)</a:t>
+            <a:t> varchar(75)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
@@ -5381,7 +5381,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t> varchar(20)</a:t>
+            <a:t> varchar(30)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
             <a:solidFill>
@@ -9023,33 +9023,33 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>96116</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>54430</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>25266</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>178996</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>118382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226623</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="73" name="Elbow Connector 72"/>
+        <xdr:cNvPr id="74" name="Elbow Connector 73"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="42" idx="1"/>
-          <a:endCxn id="48" idx="1"/>
+          <a:stCxn id="57" idx="1"/>
+          <a:endCxn id="60" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="7960180" y="4668116"/>
-          <a:ext cx="54429" cy="2405650"/>
+          <a:off x="11761396" y="6023882"/>
+          <a:ext cx="47627" cy="3514725"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 519997"/>
+            <a:gd name="adj1" fmla="val 579980"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -9075,33 +9075,33 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>178996</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>118382</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>226623</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>13607</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>492950</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>131990</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>526968</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95930</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="74" name="Elbow Connector 73"/>
+        <xdr:cNvPr id="75" name="Elbow Connector 74"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="57" idx="1"/>
-          <a:endCxn id="60" idx="1"/>
+          <a:stCxn id="51" idx="1"/>
+          <a:endCxn id="54" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="11761396" y="6023882"/>
-          <a:ext cx="47627" cy="3514725"/>
+          <a:off x="15732950" y="6989990"/>
+          <a:ext cx="34018" cy="1868940"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 579980"/>
+            <a:gd name="adj1" fmla="val 771997"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -9127,33 +9127,33 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226622</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>118382</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>492950</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>131990</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>526968</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>95930</xdr:rowOff>
+      <xdr:rowOff>95929</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="Elbow Connector 74"/>
+        <xdr:cNvPr id="76" name="Elbow Connector 75"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="51" idx="1"/>
+          <a:stCxn id="57" idx="1"/>
           <a:endCxn id="54" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="15732950" y="6989990"/>
-          <a:ext cx="34018" cy="1868940"/>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="11809022" y="6023882"/>
+          <a:ext cx="3923928" cy="2835047"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 771997"/>
+            <a:gd name="adj1" fmla="val -5826"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -9181,31 +9181,31 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>226622</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>92529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>324592</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>118382</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>492950</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>95929</xdr:rowOff>
+      <xdr:rowOff>118383</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="76" name="Elbow Connector 75"/>
+        <xdr:cNvPr id="77" name="Elbow Connector 76"/>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="57" idx="1"/>
-          <a:endCxn id="54" idx="1"/>
+          <a:endCxn id="63" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000" flipH="1" flipV="1">
-          <a:off x="11809022" y="6023882"/>
-          <a:ext cx="3923928" cy="2835047"/>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="11809022" y="3902529"/>
+          <a:ext cx="97970" cy="2121354"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -5826"/>
+            <a:gd name="adj1" fmla="val -233337"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -9231,34 +9231,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>226622</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>92529</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>324592</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>298495</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>122463</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>422442</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>118383</xdr:rowOff>
+      <xdr:rowOff>118382</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="77" name="Elbow Connector 76"/>
+        <xdr:cNvPr id="78" name="Elbow Connector 77"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="57" idx="1"/>
-          <a:endCxn id="63" idx="1"/>
+          <a:stCxn id="45" idx="1"/>
+          <a:endCxn id="57" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000" flipH="1">
-          <a:off x="11809022" y="3902529"/>
-          <a:ext cx="97970" cy="2121354"/>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="14319295" y="4313463"/>
+          <a:ext cx="1343147" cy="1710419"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -233337"/>
-          </a:avLst>
+          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -9283,29 +9281,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>298495</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>122463</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>422442</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>126300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>96117</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>226622</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>118382</xdr:rowOff>
+      <xdr:rowOff>118384</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="Elbow Connector 77"/>
+        <xdr:cNvPr id="79" name="Elbow Connector 78"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="45" idx="1"/>
-          <a:endCxn id="57" idx="3"/>
+          <a:stCxn id="57" idx="1"/>
+          <a:endCxn id="42" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="14319295" y="4313463"/>
-          <a:ext cx="1343147" cy="1710419"/>
+        <a:xfrm rot="10800000">
+          <a:off x="10489500" y="4668117"/>
+          <a:ext cx="1319522" cy="1355767"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -9333,32 +9331,184 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>126300</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>383758</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>134</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>305067</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152957</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="Text Box 11"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12506485" y="1905134"/>
+          <a:ext cx="1133582" cy="533823"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>LEGEND</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>331011</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>150165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>402882</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>162994</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="88" name="Text Box 13"/>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11847602" y="2436165"/>
+          <a:ext cx="2496416" cy="584329"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="39999"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>NULL = RED</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>NOT NULL = BLACK </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>96117</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>226622</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>118384</xdr:rowOff>
+      <xdr:rowOff>96116</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>54430</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>25266</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="79" name="Elbow Connector 78"/>
+        <xdr:cNvPr id="3" name="Elbow Connector 2"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="57" idx="1"/>
-          <a:endCxn id="42" idx="3"/>
+          <a:stCxn id="42" idx="1"/>
+          <a:endCxn id="48" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="10489500" y="4668117"/>
-          <a:ext cx="1319522" cy="1355767"/>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="7960180" y="4668116"/>
+          <a:ext cx="54429" cy="2405650"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
-          <a:avLst/>
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 519997"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="arrow"/>
@@ -9383,51 +9533,51 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>383758</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>211813</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>134</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>305067</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>163285</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>152957</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="86" name="Text Box 11"/>
+        <xdr:cNvPr id="80" name="Text Box 11"/>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12506485" y="1905134"/>
-          <a:ext cx="1133582" cy="533823"/>
+          <a:off x="15519849" y="1905134"/>
+          <a:ext cx="1788436" cy="533823"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="6350">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
+        <a:ln>
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="39999"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
         <a:lstStyle/>
@@ -9438,11 +9588,11 @@
           <a:r>
             <a:rPr lang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>LEGEND</a:t>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>Address Type</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -9451,81 +9601,101 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>331011</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>417602</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>150165</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>402882</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162994</xdr:rowOff>
+      <xdr:rowOff>150164</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>489473</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="88" name="Text Box 13"/>
+        <xdr:cNvPr id="81" name="Text Box 13"/>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11847602" y="2436165"/>
-          <a:ext cx="2496416" cy="584329"/>
+          <a:off x="15113316" y="2436164"/>
+          <a:ext cx="2521157" cy="992835"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="00B0F0"/>
-        </a:solidFill>
-        <a:ln w="6350">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
+        <a:ln>
           <a:headEnd/>
           <a:tailEnd/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="39999"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="t" upright="1"/>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" anchor="ctr" upright="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
             <a:defRPr sz="1000"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:rPr>
-            <a:t>NULL = RED</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>NOT NULL = BLACK </a:t>
-          </a:r>
+            <a:t>1 = Billing</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>2=Mailing</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:rPr>
+            <a:t>3 = Both</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Calibri"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -9839,7 +10009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J12:AB39"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
@@ -9864,8 +10034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF16" sqref="AF16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>